<commit_message>
create add request methods
</commit_message>
<xml_diff>
--- a/APIcodes.xlsx
+++ b/APIcodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\IdeaProjects\YouTube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33624077-EC63-46AC-B23E-9B11B5D160D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0206B278-364A-43BA-8D4B-50B0A6D30F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B838076E-603B-497C-A7EA-0EFC6F232AF3}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{B838076E-603B-497C-A7EA-0EFC6F232AF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>get</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>send image bytes</t>
+  </si>
+  <si>
+    <t>get saved videos</t>
+  </si>
+  <si>
+    <t>get saved playlists</t>
+  </si>
+  <si>
+    <t>get videos by random category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get video history </t>
   </si>
 </sst>
 </file>
@@ -525,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6689DA5C-8376-4AA3-A53B-E688119AAC51}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N7" sqref="M7:N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,8 +804,36 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
create update request methods
</commit_message>
<xml_diff>
--- a/APIcodes.xlsx
+++ b/APIcodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\IdeaProjects\YouTube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0206B278-364A-43BA-8D4B-50B0A6D30F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A62410D-58AE-405F-A528-25F0FAD63EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{B838076E-603B-497C-A7EA-0EFC6F232AF3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B838076E-603B-497C-A7EA-0EFC6F232AF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>get</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t xml:space="preserve">get video history </t>
+  </si>
+  <si>
+    <t>delete video comments</t>
+  </si>
+  <si>
+    <t>update video views</t>
+  </si>
+  <si>
+    <t>update video likes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update video deslike </t>
   </si>
 </sst>
 </file>
@@ -539,20 +551,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6689DA5C-8376-4AA3-A53B-E688119AAC51}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="3.88671875" customWidth="1"/>
+    <col min="3" max="3" width="1.77734375" customWidth="1"/>
     <col min="4" max="4" width="21.109375" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" customWidth="1"/>
-    <col min="8" max="8" width="3.5546875" customWidth="1"/>
+    <col min="6" max="6" width="2.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" customWidth="1"/>
+    <col min="8" max="8" width="2.77734375" customWidth="1"/>
+    <col min="9" max="9" width="2.33203125" customWidth="1"/>
     <col min="10" max="10" width="20.88671875" customWidth="1"/>
     <col min="11" max="11" width="3.77734375" customWidth="1"/>
+    <col min="12" max="12" width="2.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -716,6 +732,12 @@
       <c r="E6" s="3">
         <v>25</v>
       </c>
+      <c r="G6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="4">
+        <v>35</v>
+      </c>
       <c r="J6" s="5" t="s">
         <v>29</v>
       </c>
@@ -810,6 +832,12 @@
       <c r="B11" s="2">
         <v>110</v>
       </c>
+      <c r="J11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="5">
+        <v>410</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -818,6 +846,12 @@
       <c r="B12" s="2">
         <v>111</v>
       </c>
+      <c r="J12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="5">
+        <v>411</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -825,6 +859,12 @@
       </c>
       <c r="B13" s="2">
         <v>112</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="5">
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
create API directory create checking API
</commit_message>
<xml_diff>
--- a/APIcodes.xlsx
+++ b/APIcodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\IdeaProjects\YouTube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A62410D-58AE-405F-A528-25F0FAD63EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE18BE0C-608E-4526-8AC3-17317851C30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B838076E-603B-497C-A7EA-0EFC6F232AF3}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{B838076E-603B-497C-A7EA-0EFC6F232AF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>get</t>
   </si>
@@ -54,9 +54,6 @@
     <t>get playlist videos</t>
   </si>
   <si>
-    <t>get  videos by category</t>
-  </si>
-  <si>
     <t>add</t>
   </si>
   <si>
@@ -129,18 +126,6 @@
     <t>edit channel links</t>
   </si>
   <si>
-    <t>get video bytes</t>
-  </si>
-  <si>
-    <t>get iamge bytes</t>
-  </si>
-  <si>
-    <t>send video bytes</t>
-  </si>
-  <si>
-    <t>send image bytes</t>
-  </si>
-  <si>
     <t>get saved videos</t>
   </si>
   <si>
@@ -163,6 +148,27 @@
   </si>
   <si>
     <t xml:space="preserve">update video deslike </t>
+  </si>
+  <si>
+    <t>get videos by category</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>check email</t>
+  </si>
+  <si>
+    <t>check username</t>
+  </si>
+  <si>
+    <t>check user exists</t>
+  </si>
+  <si>
+    <t>check video saving</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> check playlist saving</t>
   </si>
 </sst>
 </file>
@@ -178,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +221,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -228,13 +240,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6689DA5C-8376-4AA3-A53B-E688119AAC51}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,6 +583,8 @@
     <col min="10" max="10" width="20.88671875" customWidth="1"/>
     <col min="11" max="11" width="3.77734375" customWidth="1"/>
     <col min="12" max="12" width="2.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="14" max="14" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -579,25 +595,25 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1">
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1">
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="N1" s="1">
         <v>5</v>
@@ -611,22 +627,28 @@
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3">
         <v>21</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="4">
         <v>31</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="5">
         <v>41</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="6">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -637,28 +659,28 @@
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>22</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="4">
         <v>32</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K3" s="5">
         <v>42</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="1">
-        <v>6</v>
+      <c r="M3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="6">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -669,22 +691,28 @@
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="3">
         <v>23</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="4">
         <v>33</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" s="5">
         <v>43</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="6">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -695,28 +723,28 @@
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="3">
         <v>24</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="4">
         <v>34</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5" s="5">
         <v>44</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="1">
-        <v>7</v>
+      <c r="M5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="6">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -727,22 +755,28 @@
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="3">
         <v>25</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H6" s="4">
         <v>35</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K6" s="5">
         <v>45</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" s="6">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -753,23 +787,19 @@
         <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="3">
         <v>26</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" s="5">
         <v>46</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="1">
-        <v>8</v>
-      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -779,13 +809,13 @@
         <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3">
         <v>27</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K8" s="5">
         <v>47</v>
@@ -799,13 +829,13 @@
         <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3">
         <v>28</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K9" s="5">
         <v>48</v>
@@ -813,13 +843,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2">
         <v>19</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K10" s="5">
         <v>49</v>
@@ -827,13 +857,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2">
         <v>110</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K11" s="5">
         <v>410</v>
@@ -841,13 +871,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2">
         <v>111</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K12" s="5">
         <v>411</v>
@@ -855,13 +885,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2">
         <v>112</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K13" s="5">
         <v>412</v>
@@ -869,7 +899,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2">
         <v>113</v>

</xml_diff>